<commit_message>
added appartment_search success day-7, 8
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -746,21 +746,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rony</t>
+          <t>Shakib Ahmed</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ujjal</t>
+          <t>Shak Forid</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">kakoli </t>
+          <t>Aklima</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>234567</v>
+        <v>677287</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -769,12 +769,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Electronics Technology (68)</t>
+          <t>Computer Science &amp; Technology (85)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>23/05/2007</t>
+          <t>23/06/2003</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">

</xml_diff>

<commit_message>
added mcq and reduce icons size day - 10
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -803,6 +803,69 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>107</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Shakib</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Shak Forid</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Aklima</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>677287</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Computer Science &amp; Technology (85)</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>23/06/2003</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Habiganj Polytechnic Institute (63010)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Gopaya</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Habiganj Sadar</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Habiganj</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>2021-22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>